<commit_message>
updated max gest from 301 to 308
</commit_message>
<xml_diff>
--- a/inst/concepts/Matcho_term_durations.xlsx
+++ b/inst/concepts/Matcho_term_durations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonesse3/Desktop/n3c_preg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Packages\PregnancyIdentifier\inst\concepts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF07A4C9-0E18-164E-BC83-7C7454461A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FE5E6E-8B1E-4676-ACF1-0EDC170A89F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{7713BFDA-036C-8940-8938-64F83783E9E6}"/>
+    <workbookView xWindow="-5652" yWindow="6384" windowWidth="23232" windowHeight="13872" xr2:uid="{7713BFDA-036C-8940-8938-64F83783E9E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,10 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,9 +129,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -170,7 +169,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -276,7 +275,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -418,7 +417,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -426,18 +425,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9882890-62D5-9C47-9622-F1DD2CD4AC96}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="10.83203125" style="2"/>
+    <col min="1" max="5" width="10.875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -451,87 +450,87 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>301</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2">
+        <v>308</v>
+      </c>
+      <c r="C2">
         <v>140</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>84</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>42</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>168</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>42</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
-        <v>301</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5">
+        <v>308</v>
+      </c>
+      <c r="C5">
         <v>161</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
-        <v>301</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6">
+        <v>308</v>
+      </c>
+      <c r="C6">
         <v>140</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>139</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>28</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>14</v>
       </c>
     </row>

</xml_diff>